<commit_message>
added notebook to plot results
</commit_message>
<xml_diff>
--- a/Assignment5/results.xlsx
+++ b/Assignment5/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marlan/Documents/Github/STA5635/Assignment5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2889142E-AA03-184D-9CC5-B84B698B441A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7A48E8-F7B3-4541-92F9-6A69B410837B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15740" xr2:uid="{D9B13871-FA45-214C-8673-2D05CDAA2C91}"/>
   </bookViews>
@@ -527,185 +527,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7BD02C-958C-D54A-9A74-89BD4A255ADE}">
-  <dimension ref="B2:E13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2">
+      <c r="B2" s="2">
         <v>5.13</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C2" s="2">
         <v>31.31</v>
       </c>
-      <c r="E3" s="1">
+      <c r="D2" s="1">
         <v>2.94</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>25.16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10.71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
       <c r="C4" s="3">
+        <v>24.99</v>
+      </c>
+      <c r="D4" s="1">
+        <v>32.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3">
+        <v>28.71</v>
+      </c>
+      <c r="C5" s="3">
+        <v>40.450000000000003</v>
+      </c>
+      <c r="D5" s="1">
+        <v>41.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3">
+        <v>33.93</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45.73</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="3">
-        <v>25.16</v>
-      </c>
-      <c r="E4" s="1">
-        <v>10.71</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="C7" s="3">
+        <v>24.69</v>
+      </c>
+      <c r="D7" s="1">
+        <v>48.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="3">
-        <v>24.99</v>
-      </c>
-      <c r="E5" s="1">
-        <v>32.49</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3">
-        <v>28.71</v>
-      </c>
-      <c r="D6" s="3">
-        <v>40.450000000000003</v>
-      </c>
-      <c r="E6" s="1">
-        <v>41.11</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3">
-        <v>33.93</v>
-      </c>
-      <c r="D7" s="3">
-        <v>45.73</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C8" s="3">
+        <v>22.87</v>
+      </c>
+      <c r="D8" s="1">
+        <v>237.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>29.15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>48.16</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.5399999999999991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>21.8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>38.86</v>
+      </c>
+      <c r="D10" s="1">
+        <v>94.26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3">
+        <v>21.31</v>
+      </c>
+      <c r="C11" s="3">
+        <v>39.26</v>
+      </c>
+      <c r="D11" s="1">
+        <v>29.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5">
         <v>0</v>
       </c>
-      <c r="D8" s="3">
-        <v>24.69</v>
-      </c>
-      <c r="E8" s="1">
-        <v>48.99</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>22.87</v>
-      </c>
-      <c r="E9" s="1">
-        <v>237.88</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3">
-        <v>29.15</v>
-      </c>
-      <c r="D10" s="3">
-        <v>48.16</v>
-      </c>
-      <c r="E10" s="1">
-        <v>9.5399999999999991</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3">
-        <v>21.8</v>
-      </c>
-      <c r="D11" s="3">
-        <v>38.86</v>
-      </c>
-      <c r="E11" s="1">
-        <v>94.26</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3">
-        <v>21.31</v>
-      </c>
-      <c r="D12" s="3">
-        <v>39.26</v>
-      </c>
-      <c r="E12" s="1">
-        <v>29.04</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="C12" s="5">
         <v>23.62</v>
       </c>
-      <c r="E13" s="6">
+      <c r="D12" s="6">
         <v>332.71</v>
       </c>
     </row>

</xml_diff>